<commit_message>
Update AccountDetails and AccountStatement features
</commit_message>
<xml_diff>
--- a/src/assets/對帳單明細.xlsx
+++ b/src/assets/對帳單明細.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\G-Tai\G-Tai\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\G-Tai-client\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -116,31 +116,99 @@
     </r>
   </si>
   <si>
-    <t>帳單期別：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>車牌號碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交易日期時間</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>產品名稱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>售價金額</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>單價</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>數量</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+      </rPr>
+      <t>帳單期別：</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>車牌號碼</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>交易日期時間</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>產品名稱</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>單價</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>數量</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+      </rPr>
+      <t>售價金額</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -239,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -256,40 +324,31 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -635,107 +694,107 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.25" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.25" style="12" customWidth="1"/>
     <col min="4" max="4" width="12.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.75" style="11" customWidth="1"/>
-    <col min="6" max="6" width="9.375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="7.375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="8.75" style="10" customWidth="1"/>
+    <col min="6" max="6" width="9.375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="7.375" style="11" customWidth="1"/>
     <col min="8" max="9" width="13.375" style="2" customWidth="1"/>
     <col min="10" max="10" width="14.75" style="2" customWidth="1"/>
     <col min="11" max="16384" width="8.75" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="9"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>11</v>
+      <c r="I6" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>6</v>

</xml_diff>